<commit_message>
Update to include demo of file request functionality.
</commit_message>
<xml_diff>
--- a/CITS-WebService/Documentation/APEXA CITS Documentation.xlsx
+++ b/CITS-WebService/Documentation/APEXA CITS Documentation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="456">
   <si>
     <t>ACORD Hierarchy</t>
   </si>
@@ -929,9 +929,6 @@
     <t>TXLifeResponse/OLifE/Holding[N]/Loan/@FinancialInstitutionPartyID</t>
   </si>
   <si>
-    <t>TXLifeResponse/OLifE/Party[1]/Producer/CarrierAppointment[N]/TermDate</t>
-  </si>
-  <si>
     <t>Date the contract was terminated.  Not provided unless the contract was terminated.</t>
   </si>
   <si>
@@ -1196,14 +1193,6 @@
   </si>
   <si>
     <t>Will be the APEXA EntityId prefixed with the letters "CON"</t>
-  </si>
-  <si>
-    <t>Points to the AGA MGA or Carrier that this contract is with.  In the case of multi-level contracts it is the highest tier (Carrier &gt; MGA &gt; AGA)
-Will be the APEXA EntityId prefixed with the letters "P"</t>
-  </si>
-  <si>
-    <t>Will be the APEXA EntityId prefixed with the letters "P"
-References the contract being transferred.</t>
   </si>
   <si>
     <t>Will be the APEXA Contract EntityId prefixed with the letters "REF"</t>
@@ -1489,9 +1478,6 @@
 OLI_REL_EMPLOYEE - 6 - Employee</t>
   </si>
   <si>
-    <t>TXLifeResponse/OLifE/Party[1]/Producer/CarrierAppointment[N]/TransferInfo/CarrierAppointmentID</t>
-  </si>
-  <si>
     <t>TXLifeResponse/OLifE/Party[1]/Producer/CarrierAppointment[N]/RequirementInfo/Attachment/FileName</t>
   </si>
   <si>
@@ -1515,7 +1501,36 @@
     <t>Will be the APEXA AddressID prefixed with "ADR"</t>
   </si>
   <si>
-    <t>Will be the APEXA EntityId prefixed with the letters "CONSD"</t>
+    <t>TXLifeResponse/OLifE/Party[1]/Producer/CarrierAppointment[N]/ExpDate</t>
+  </si>
+  <si>
+    <t>TXLifeResponse/OLifE/Party[1]/Producer/CarrierAppointment[N]/AssocCarrierApptInfo/@PartyID</t>
+  </si>
+  <si>
+    <t>TXLifeResponse/OLifE/Party[1]/Producer/CarrierAppointment[N]/AssocCarrierApptInfo/CompanyProducerID</t>
+  </si>
+  <si>
+    <t>TXLifeResponse/OLifE/Party[1]/Producer/CarrierAppointment[N]/AssocCarrierApptInfo/CarrierApptStatus</t>
+  </si>
+  <si>
+    <t>Represents the state of the associated contract.
+As far as APEXA is concerned the CITS Transfer Out status is used to represent that a contract has been transfered to either another company OR another contract within the same company.
+APEXA will only have the notion of a "Downgraded" contract which can be interpretted by the corresponding carrier/mga as per their internal business rules (Included here as 7 - Servicing Only)</t>
+  </si>
+  <si>
+    <t>TXLifeResponse/OLifE/Party[1]/Producer/CarrierAppointment[N]/AssocCarrierApptInfo/@CarrierAppointmentID</t>
+  </si>
+  <si>
+    <t>Will be the APEXA EntityId prefixed with the letters "CON"
+References the contract being transferred.</t>
+  </si>
+  <si>
+    <t>Points to the AGA ,MGA or Carrier that this contract is with.
+Will be the APEXA EntityId prefixed with the letters "P"</t>
+  </si>
+  <si>
+    <t>Points to the AGA, MGA or Carrier that this contract is with.  In the case of multi-level contracts it is the highest tier (Carrier &gt; MGA &gt; AGA)
+Will be the APEXA EntityId prefixed with the letters "P"</t>
   </si>
 </sst>
 </file>
@@ -1979,7 +1994,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2026,6 +2041,12 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2047,13 +2068,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2435,7 +2456,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="5" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
@@ -2454,60 +2475,60 @@
         <v>89</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>179</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="6" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>335</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="12" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="12" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>250</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
@@ -2519,7 +2540,7 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2863,7 +2884,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="11" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
@@ -2911,12 +2932,12 @@
       </c>
     </row>
     <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
     </row>
     <row r="8" spans="1:4" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -2926,7 +2947,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="11" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
@@ -2937,7 +2958,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="11" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
@@ -2953,13 +2974,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2970,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -2986,10 +3007,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M293"/>
+  <dimension ref="A1:M296"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="4" x14ac:dyDescent="0.25"/>
@@ -3035,7 +3056,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
@@ -3092,12 +3113,12 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
@@ -3118,7 +3139,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="22.5" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3150,8 +3171,8 @@
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="22" t="s">
-        <v>409</v>
+      <c r="D13" s="24" t="s">
+        <v>406</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -3171,9 +3192,9 @@
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="D14" s="22"/>
+        <v>405</v>
+      </c>
+      <c r="D14" s="24"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
@@ -3191,7 +3212,7 @@
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="24" t="s">
         <v>181</v>
       </c>
       <c r="E15" s="15"/>
@@ -3211,7 +3232,7 @@
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
@@ -3232,7 +3253,7 @@
       <c r="C17" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -3310,7 +3331,7 @@
         <v>104</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -3348,7 +3369,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="30" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3364,10 +3385,10 @@
     </row>
     <row r="31" spans="1:13" s="14" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -3416,7 +3437,7 @@
     </row>
     <row r="36" spans="1:13" ht="146.25" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>55</v>
@@ -3427,13 +3448,13 @@
     </row>
     <row r="37" spans="1:13" s="14" customFormat="1" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -3478,24 +3499,24 @@
     </row>
     <row r="40" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="41" spans="1:13" s="14" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B41" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
@@ -3523,7 +3544,7 @@
         <v>21</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="44" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -3544,7 +3565,7 @@
     </row>
     <row r="46" spans="1:13" s="14" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>3</v>
@@ -3583,7 +3604,7 @@
         <v>22</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="50" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -3596,13 +3617,13 @@
     </row>
     <row r="51" spans="1:13" s="7" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="E51" s="15"/>
       <c r="F51" s="15"/>
@@ -3616,13 +3637,13 @@
     </row>
     <row r="52" spans="1:13" s="8" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="E52" s="15"/>
       <c r="F52" s="15"/>
@@ -3636,7 +3657,7 @@
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>253</v>
@@ -3656,13 +3677,13 @@
     </row>
     <row r="54" spans="1:13" s="10" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E54" s="15"/>
       <c r="F54" s="15"/>
@@ -3676,13 +3697,13 @@
     </row>
     <row r="55" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="15"/>
@@ -3696,7 +3717,7 @@
     </row>
     <row r="56" spans="1:13" s="14" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>3</v>
@@ -3732,7 +3753,7 @@
     </row>
     <row r="59" spans="1:13" s="14" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>23</v>
@@ -3776,12 +3797,12 @@
       <c r="M61" s="15"/>
     </row>
     <row r="62" spans="1:13" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
     </row>
     <row r="63" spans="1:13" ht="33.75" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
@@ -3807,13 +3828,13 @@
     </row>
     <row r="65" spans="1:13" s="14" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B65" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="66" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -3828,12 +3849,12 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
     </row>
     <row r="68" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
@@ -3843,18 +3864,18 @@
         <v>10</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="69" spans="1:13" s="11" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B69" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E69" s="15"/>
       <c r="F69" s="15"/>
@@ -3874,7 +3895,7 @@
         <v>12</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="71" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -3885,18 +3906,18 @@
         <v>3</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="72" spans="1:13" s="14" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B72" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="146.25" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -3924,7 +3945,7 @@
         <v>54</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="75" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -3935,18 +3956,18 @@
         <v>12</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="76" spans="1:13" s="14" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B76" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E76" s="15"/>
       <c r="F76" s="15"/>
@@ -3959,12 +3980,12 @@
       <c r="M76" s="15"/>
     </row>
     <row r="77" spans="1:13" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+      <c r="A77" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
     </row>
     <row r="78" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
@@ -3988,7 +4009,7 @@
         <v>75</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="80" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4010,7 +4031,7 @@
         <v>3</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="82" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4021,16 +4042,16 @@
         <v>12</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="16" t="s">
+      <c r="A83" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B83" s="17"/>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
     </row>
     <row r="84" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
@@ -4068,7 +4089,7 @@
         <v>10</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="87" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4083,12 +4104,12 @@
       </c>
     </row>
     <row r="88" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="16" t="s">
+      <c r="A88" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="B88" s="17"/>
-      <c r="C88" s="17"/>
-      <c r="D88" s="17"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
     </row>
     <row r="89" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
@@ -4143,12 +4164,12 @@
       </c>
     </row>
     <row r="94" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
+      <c r="A94" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B94" s="17"/>
-      <c r="C94" s="17"/>
-      <c r="D94" s="17"/>
+      <c r="B94" s="19"/>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19"/>
     </row>
     <row r="95" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
@@ -4169,7 +4190,7 @@
         <v>11</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="97" spans="1:4" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4256,7 +4277,7 @@
         <v>11</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4267,7 +4288,7 @@
         <v>23</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4278,7 +4299,7 @@
         <v>23</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="108" spans="1:4" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4315,12 +4336,12 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="16" t="s">
+      <c r="A111" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B111" s="17"/>
-      <c r="C111" s="17"/>
-      <c r="D111" s="17"/>
+      <c r="B111" s="19"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19"/>
     </row>
     <row r="112" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
@@ -4368,7 +4389,7 @@
         <v>3</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="117" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4379,7 +4400,7 @@
         <v>3</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="118" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4401,7 +4422,7 @@
         <v>65</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="120" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4412,7 +4433,7 @@
         <v>12</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="121" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4423,7 +4444,7 @@
         <v>12</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="122" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4434,7 +4455,7 @@
         <v>12</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="123" spans="1:13" ht="45" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4448,7 +4469,7 @@
         <v>72</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="124" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4459,7 +4480,7 @@
         <v>10</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="125" spans="1:13" s="2" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4470,7 +4491,7 @@
         <v>69</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="E125" s="15"/>
       <c r="F125" s="15"/>
@@ -4523,7 +4544,7 @@
     </row>
     <row r="129" spans="1:13" s="14" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B129" s="14" t="s">
         <v>3</v>
@@ -4580,12 +4601,12 @@
       </c>
     </row>
     <row r="134" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A134" s="16" t="s">
+      <c r="A134" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B134" s="17"/>
-      <c r="C134" s="17"/>
-      <c r="D134" s="17"/>
+      <c r="B134" s="19"/>
+      <c r="C134" s="19"/>
+      <c r="D134" s="19"/>
     </row>
     <row r="135" spans="1:13" s="2" customFormat="1" ht="22.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
@@ -4615,7 +4636,7 @@
         <v>11</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E136" s="15"/>
       <c r="F136" s="15"/>
@@ -4649,7 +4670,7 @@
         <v>60</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="139" spans="1:13" s="11" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4660,7 +4681,7 @@
         <v>59</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E139" s="15"/>
       <c r="F139" s="15"/>
@@ -4674,16 +4695,16 @@
     </row>
     <row r="140" spans="1:13" s="11" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B140" s="11" t="s">
         <v>250</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E140" s="15"/>
       <c r="F140" s="15"/>
@@ -4697,13 +4718,13 @@
     </row>
     <row r="141" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>250</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="142" spans="1:13" s="7" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4734,7 +4755,7 @@
         <v>11</v>
       </c>
       <c r="D143" s="7" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E143" s="15"/>
       <c r="F143" s="15"/>
@@ -4754,7 +4775,7 @@
         <v>23</v>
       </c>
       <c r="D144" s="7" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E144" s="15"/>
       <c r="F144" s="15"/>
@@ -4774,7 +4795,7 @@
         <v>23</v>
       </c>
       <c r="D145" s="7" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E145" s="15"/>
       <c r="F145" s="15"/>
@@ -4847,12 +4868,12 @@
       <c r="M148" s="15"/>
     </row>
     <row r="149" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A149" s="16" t="s">
-        <v>399</v>
-      </c>
-      <c r="B149" s="17"/>
-      <c r="C149" s="17"/>
-      <c r="D149" s="17"/>
+      <c r="A149" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="B149" s="19"/>
+      <c r="C149" s="19"/>
+      <c r="D149" s="19"/>
     </row>
     <row r="150" spans="1:13" ht="22.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A150" s="15" t="s">
@@ -4862,7 +4883,7 @@
         <v>10</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="151" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4912,18 +4933,18 @@
         <v>23</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="155" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A155" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B155" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="B155" s="7" t="s">
+      <c r="C155" s="7" t="s">
         <v>287</v>
-      </c>
-      <c r="C155" s="7" t="s">
-        <v>288</v>
       </c>
       <c r="E155" s="15"/>
       <c r="F155" s="15"/>
@@ -4937,13 +4958,13 @@
     </row>
     <row r="156" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A156" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B156" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D156" s="7" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E156" s="15"/>
       <c r="F156" s="15"/>
@@ -4963,7 +4984,7 @@
         <v>65</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="158" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4973,7 +4994,7 @@
       <c r="B158" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D158" s="20" t="s">
+      <c r="D158" s="22" t="s">
         <v>193</v>
       </c>
     </row>
@@ -4984,7 +5005,7 @@
       <c r="B159" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D159" s="21"/>
+      <c r="D159" s="23"/>
     </row>
     <row r="160" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A160" s="15" t="s">
@@ -4996,7 +5017,7 @@
       <c r="C160" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D160" s="21"/>
+      <c r="D160" s="23"/>
     </row>
     <row r="161" spans="1:13" ht="11.25" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A161" s="15" t="s">
@@ -5005,7 +5026,7 @@
       <c r="B161" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D161" s="21"/>
+      <c r="D161" s="23"/>
     </row>
     <row r="162" spans="1:13" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A162" s="15" t="s">
@@ -5035,7 +5056,7 @@
         <v>11</v>
       </c>
       <c r="D163" s="7" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E163" s="15"/>
       <c r="F163" s="15"/>
@@ -5075,7 +5096,7 @@
         <v>23</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E165" s="15"/>
       <c r="F165" s="15"/>
@@ -5151,12 +5172,12 @@
       <c r="M168" s="15"/>
     </row>
     <row r="169" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A169" s="16" t="s">
+      <c r="A169" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B169" s="17"/>
-      <c r="C169" s="17"/>
-      <c r="D169" s="17"/>
+      <c r="B169" s="19"/>
+      <c r="C169" s="19"/>
+      <c r="D169" s="19"/>
     </row>
     <row r="170" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
@@ -5177,7 +5198,7 @@
         <v>11</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
     </row>
     <row r="172" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5218,7 +5239,7 @@
         <v>11</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="176" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5229,7 +5250,7 @@
         <v>23</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5240,7 +5261,7 @@
         <v>23</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="178" spans="1:4" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5277,20 +5298,20 @@
       </c>
     </row>
     <row r="181" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A181" s="16" t="s">
+      <c r="A181" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B181" s="17"/>
-      <c r="C181" s="17"/>
-      <c r="D181" s="17"/>
+      <c r="B181" s="19"/>
+      <c r="C181" s="19"/>
+      <c r="D181" s="19"/>
     </row>
     <row r="182" spans="1:4" s="14" customFormat="1" ht="42.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="18" t="s">
+      <c r="A182" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="B182" s="19"/>
-      <c r="C182" s="19"/>
-      <c r="D182" s="19"/>
+      <c r="B182" s="21"/>
+      <c r="C182" s="21"/>
+      <c r="D182" s="21"/>
     </row>
     <row r="183" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
@@ -5311,7 +5332,7 @@
         <v>11</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -5322,7 +5343,7 @@
         <v>23</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -5333,7 +5354,7 @@
         <v>23</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="187" spans="1:4" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -5366,7 +5387,7 @@
         <v>35</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="190" spans="1:4" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -5381,12 +5402,12 @@
       </c>
     </row>
     <row r="191" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A191" s="16" t="s">
-        <v>333</v>
-      </c>
-      <c r="B191" s="17"/>
-      <c r="C191" s="17"/>
-      <c r="D191" s="17"/>
+      <c r="A191" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="B191" s="19"/>
+      <c r="C191" s="19"/>
+      <c r="D191" s="19"/>
     </row>
     <row r="192" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A192" s="14" t="s">
@@ -5407,7 +5428,7 @@
         <v>11</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="194" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5418,7 +5439,7 @@
         <v>23</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="195" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5429,7 +5450,7 @@
         <v>23</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="196" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5462,7 +5483,7 @@
         <v>35</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="199" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5495,7 +5516,7 @@
         <v>11</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="202" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5506,7 +5527,7 @@
         <v>7</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="203" spans="1:13" s="11" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5528,7 +5549,7 @@
     </row>
     <row r="204" spans="1:13" s="11" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A204" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B204" s="11" t="s">
         <v>10</v>
@@ -5545,19 +5566,19 @@
     </row>
     <row r="205" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A205" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="206" spans="1:13" s="7" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="16" t="s">
-        <v>283</v>
-      </c>
-      <c r="B206" s="17"/>
-      <c r="C206" s="17"/>
-      <c r="D206" s="17"/>
+      <c r="A206" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="B206" s="19"/>
+      <c r="C206" s="19"/>
+      <c r="D206" s="19"/>
       <c r="E206" s="15"/>
       <c r="F206" s="15"/>
       <c r="G206" s="15"/>
@@ -5573,7 +5594,7 @@
         <v>201</v>
       </c>
       <c r="D207" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E207" s="15"/>
       <c r="F207" s="15"/>
@@ -5593,7 +5614,7 @@
         <v>11</v>
       </c>
       <c r="D208" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E208" s="15"/>
       <c r="F208" s="15"/>
@@ -5613,7 +5634,7 @@
         <v>3</v>
       </c>
       <c r="D209" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E209" s="15"/>
       <c r="F209" s="15"/>
@@ -5666,12 +5687,12 @@
       <c r="M211" s="15"/>
     </row>
     <row r="212" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A212" s="16" t="s">
-        <v>298</v>
-      </c>
-      <c r="B212" s="17"/>
-      <c r="C212" s="17"/>
-      <c r="D212" s="17"/>
+      <c r="A212" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="B212" s="19"/>
+      <c r="C212" s="19"/>
+      <c r="D212" s="19"/>
     </row>
     <row r="213" spans="1:13" s="8" customFormat="1" ht="22.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A213" s="15" t="s">
@@ -5698,7 +5719,7 @@
         <v>231</v>
       </c>
       <c r="D214" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E214" s="15"/>
       <c r="F214" s="15"/>
@@ -5715,7 +5736,7 @@
         <v>263</v>
       </c>
       <c r="D215" s="7" t="s">
-        <v>358</v>
+        <v>455</v>
       </c>
       <c r="E215" s="15"/>
       <c r="F215" s="15"/>
@@ -5732,7 +5753,7 @@
         <v>264</v>
       </c>
       <c r="D216" s="15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="217" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5748,223 +5769,211 @@
     </row>
     <row r="218" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A218" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B218" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D218" s="15" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" s="15" customFormat="1" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A219" s="15" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="219" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A219" s="15" t="s">
-        <v>443</v>
+      <c r="B219" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="D219" s="15" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="220" spans="1:13" s="15" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" s="15" customFormat="1" ht="67.5" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A220" s="15" t="s">
-        <v>310</v>
+        <v>232</v>
       </c>
       <c r="B220" s="15" t="s">
-        <v>23</v>
+        <v>185</v>
+      </c>
+      <c r="C220" s="15" t="s">
+        <v>418</v>
       </c>
       <c r="D220" s="15" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="221" spans="1:13" s="15" customFormat="1" ht="67.5" outlineLevel="2" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A221" s="15" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B221" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="C221" s="15" t="s">
-        <v>421</v>
+        <v>12</v>
       </c>
       <c r="D221" s="15" t="s">
-        <v>422</v>
+        <v>85</v>
       </c>
     </row>
     <row r="222" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A222" s="15" t="s">
-        <v>233</v>
+        <v>447</v>
       </c>
       <c r="B222" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D222" s="15" t="s">
-        <v>85</v>
+        <v>278</v>
       </c>
     </row>
     <row r="223" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A223" s="15" t="s">
-        <v>278</v>
+        <v>304</v>
       </c>
       <c r="B223" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D223" s="15" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="224" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" s="15" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A224" s="15" t="s">
         <v>305</v>
       </c>
       <c r="B224" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D224" s="15" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" s="17" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A225" s="17" t="s">
+        <v>448</v>
+      </c>
+      <c r="B225" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D225" s="16" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" s="17" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A226" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="B226" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D226" s="17" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" s="17" customFormat="1" ht="67.5" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A227" s="17" t="s">
+        <v>450</v>
+      </c>
+      <c r="B227" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="C227" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="D227" s="17" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" s="17" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A228" s="17" t="s">
+        <v>452</v>
+      </c>
+      <c r="B228" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D228" s="17" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A229" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="B229" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D224" s="15" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="225" spans="1:13" s="15" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A225" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="B225" s="15" t="s">
+      <c r="D229" s="15" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" s="15" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A230" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="B230" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D225" s="15" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="226" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A226" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="B226" s="15" t="s">
+      <c r="D230" s="15" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A231" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B231" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D226" s="15" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="227" spans="1:13" s="15" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A227" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="B227" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D227" s="15" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="228" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A228" s="15" t="s">
+      <c r="D231" s="15" t="s">
         <v>311</v>
-      </c>
-      <c r="B228" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D228" s="15" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="229" spans="1:13" s="15" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A229" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="B229" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D229" s="15" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="230" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A230" s="15" t="s">
-        <v>411</v>
-      </c>
-      <c r="B230" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D230" s="15" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="231" spans="1:13" s="15" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A231" s="15" t="s">
-        <v>412</v>
-      </c>
-      <c r="B231" s="15" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="232" spans="1:13" s="15" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A232" s="15" t="s">
-        <v>413</v>
+        <v>319</v>
       </c>
       <c r="B232" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D232" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A233" s="15" t="s">
+        <v>408</v>
+      </c>
+      <c r="B233" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D233" s="15" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" s="15" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A234" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="B234" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" s="15" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A235" s="15" t="s">
+        <v>410</v>
+      </c>
+      <c r="B235" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C232" s="15" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="233" spans="1:13" s="2" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A233" s="15" t="s">
+      <c r="C235" s="15" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" s="2" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A236" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="B233" s="2" t="s">
+      <c r="B236" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E233" s="15"/>
-      <c r="F233" s="15"/>
-      <c r="G233" s="15"/>
-      <c r="H233" s="15"/>
-      <c r="I233" s="15"/>
-      <c r="J233" s="15"/>
-      <c r="K233" s="15"/>
-      <c r="L233" s="15"/>
-      <c r="M233" s="15"/>
-    </row>
-    <row r="234" spans="1:13" s="2" customFormat="1" ht="33.75" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A234" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D234" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E234" s="15"/>
-      <c r="F234" s="15"/>
-      <c r="G234" s="15"/>
-      <c r="H234" s="15"/>
-      <c r="I234" s="15"/>
-      <c r="J234" s="15"/>
-      <c r="K234" s="15"/>
-      <c r="L234" s="15"/>
-      <c r="M234" s="15"/>
-    </row>
-    <row r="235" spans="1:13" s="15" customFormat="1" ht="33.75" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A235" s="15" t="s">
-        <v>446</v>
-      </c>
-      <c r="B235" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D235" s="15" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="236" spans="1:13" s="2" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A236" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="B236" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C236" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="E236" s="15"/>
       <c r="F236" s="15"/>
@@ -5976,15 +5985,15 @@
       <c r="L236" s="15"/>
       <c r="M236" s="15"/>
     </row>
-    <row r="237" spans="1:13" s="13" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" s="2" customFormat="1" ht="33.75" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A237" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="B237" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D237" s="22" t="s">
-        <v>419</v>
+        <v>248</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D237" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="E237" s="15"/>
       <c r="F237" s="15"/>
@@ -5996,145 +6005,160 @@
       <c r="L237" s="15"/>
       <c r="M237" s="15"/>
     </row>
-    <row r="238" spans="1:13" s="13" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" s="15" customFormat="1" ht="33.75" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A238" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="B238" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D238" s="15" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" s="2" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A239" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E239" s="15"/>
+      <c r="F239" s="15"/>
+      <c r="G239" s="15"/>
+      <c r="H239" s="15"/>
+      <c r="I239" s="15"/>
+      <c r="J239" s="15"/>
+      <c r="K239" s="15"/>
+      <c r="L239" s="15"/>
+      <c r="M239" s="15"/>
+    </row>
+    <row r="240" spans="1:13" s="13" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A240" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B240" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D240" s="24" t="s">
         <v>416</v>
       </c>
-      <c r="B238" s="13" t="s">
+      <c r="E240" s="15"/>
+      <c r="F240" s="15"/>
+      <c r="G240" s="15"/>
+      <c r="H240" s="15"/>
+      <c r="I240" s="15"/>
+      <c r="J240" s="15"/>
+      <c r="K240" s="15"/>
+      <c r="L240" s="15"/>
+      <c r="M240" s="15"/>
+    </row>
+    <row r="241" spans="1:13" s="13" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A241" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B241" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="C241" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D241" s="23"/>
+      <c r="E241" s="15"/>
+      <c r="F241" s="15"/>
+      <c r="G241" s="15"/>
+      <c r="H241" s="15"/>
+      <c r="I241" s="15"/>
+      <c r="J241" s="15"/>
+      <c r="K241" s="15"/>
+      <c r="L241" s="15"/>
+      <c r="M241" s="15"/>
+    </row>
+    <row r="242" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A242" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" ht="45" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A243" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D243" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="C238" s="13" t="s">
-        <v>418</v>
-      </c>
-      <c r="D238" s="21"/>
-      <c r="E238" s="15"/>
-      <c r="F238" s="15"/>
-      <c r="G238" s="15"/>
-      <c r="H238" s="15"/>
-      <c r="I238" s="15"/>
-      <c r="J238" s="15"/>
-      <c r="K238" s="15"/>
-      <c r="L238" s="15"/>
-      <c r="M238" s="15"/>
-    </row>
-    <row r="239" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A239" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="B239" s="3" t="s">
+    </row>
+    <row r="244" spans="1:13" ht="11.25" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A244" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D244" s="22" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" ht="11.25" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A245" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D245" s="23"/>
+    </row>
+    <row r="246" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A246" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="B246" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D239" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="240" spans="1:13" ht="45" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A240" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="B240" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D240" s="3" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="241" spans="1:13" ht="11.25" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A241" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="B241" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D241" s="20" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="242" spans="1:13" ht="11.25" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A242" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="B242" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D242" s="21"/>
-    </row>
-    <row r="243" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A243" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="B243" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="244" spans="1:13" s="8" customFormat="1" ht="22.5" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A244" s="15" t="s">
+    </row>
+    <row r="247" spans="1:13" s="8" customFormat="1" ht="22.5" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A247" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="B244" s="8" t="s">
+      <c r="B247" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="C244" s="8" t="s">
+      <c r="C247" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="E244" s="15"/>
-      <c r="F244" s="15"/>
-      <c r="G244" s="15"/>
-      <c r="H244" s="15"/>
-      <c r="I244" s="15"/>
-      <c r="J244" s="15"/>
-      <c r="K244" s="15"/>
-      <c r="L244" s="15"/>
-      <c r="M244" s="15"/>
-    </row>
-    <row r="245" spans="1:13" s="2" customFormat="1" ht="22.5" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A245" s="15" t="s">
+      <c r="E247" s="15"/>
+      <c r="F247" s="15"/>
+      <c r="G247" s="15"/>
+      <c r="H247" s="15"/>
+      <c r="I247" s="15"/>
+      <c r="J247" s="15"/>
+      <c r="K247" s="15"/>
+      <c r="L247" s="15"/>
+      <c r="M247" s="15"/>
+    </row>
+    <row r="248" spans="1:13" s="2" customFormat="1" ht="22.5" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A248" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B245" s="2" t="s">
+      <c r="B248" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C245" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="D245" s="2" t="s">
+      <c r="C248" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="D248" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="E245" s="15"/>
-      <c r="F245" s="15"/>
-      <c r="G245" s="15"/>
-      <c r="H245" s="15"/>
-      <c r="I245" s="15"/>
-      <c r="J245" s="15"/>
-      <c r="K245" s="15"/>
-      <c r="L245" s="15"/>
-      <c r="M245" s="15"/>
-    </row>
-    <row r="246" spans="1:13" ht="22.5" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A246" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="B246" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C246" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="247" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A247" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="B247" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="248" spans="1:13" s="14" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A248" s="15" t="s">
-        <v>444</v>
-      </c>
-      <c r="B248" s="14" t="s">
-        <v>3</v>
       </c>
       <c r="E248" s="15"/>
       <c r="F248" s="15"/>
@@ -6146,122 +6170,98 @@
       <c r="L248" s="15"/>
       <c r="M248" s="15"/>
     </row>
-    <row r="249" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" ht="22.5" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A249" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="B249" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C249" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A250" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="B250" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" s="14" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A251" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="B251" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E251" s="15"/>
+      <c r="F251" s="15"/>
+      <c r="G251" s="15"/>
+      <c r="H251" s="15"/>
+      <c r="I251" s="15"/>
+      <c r="J251" s="15"/>
+      <c r="K251" s="15"/>
+      <c r="L251" s="15"/>
+      <c r="M251" s="15"/>
+    </row>
+    <row r="252" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A252" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="B249" s="3" t="s">
+      <c r="B252" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D249" s="3" t="s">
+      <c r="D252" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="250" spans="1:13" ht="33.75" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A250" s="15" t="s">
+    <row r="253" spans="1:13" ht="33.75" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A253" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="B250" s="3" t="s">
+      <c r="B253" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D250" s="3" t="s">
+      <c r="D253" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" ht="33.75" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A254" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="B254" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D254" s="3" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="251" spans="1:13" ht="33.75" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A251" s="15" t="s">
-        <v>445</v>
-      </c>
-      <c r="B251" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D251" s="3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="252" spans="1:13" ht="22.5" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A252" s="15" t="s">
+    <row r="255" spans="1:13" ht="22.5" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A255" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="B252" s="3" t="s">
+      <c r="B255" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="253" spans="1:13" ht="22.5" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A253" s="15" t="s">
+    <row r="256" spans="1:13" ht="22.5" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A256" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="B253" s="3" t="s">
+      <c r="B256" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="254" spans="1:13" s="9" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A254" s="25" t="s">
-        <v>299</v>
-      </c>
-      <c r="B254" s="24"/>
-      <c r="C254" s="24"/>
-      <c r="D254" s="24"/>
-      <c r="E254" s="15"/>
-      <c r="F254" s="15"/>
-      <c r="G254" s="15"/>
-      <c r="H254" s="15"/>
-      <c r="I254" s="15"/>
-      <c r="J254" s="15"/>
-      <c r="K254" s="15"/>
-      <c r="L254" s="15"/>
-      <c r="M254" s="15"/>
-    </row>
-    <row r="255" spans="1:13" s="7" customFormat="1" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A255" s="14" t="s">
-        <v>321</v>
-      </c>
-      <c r="B255" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D255" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="E255" s="15"/>
-      <c r="F255" s="15"/>
-      <c r="G255" s="15"/>
-      <c r="H255" s="15"/>
-      <c r="I255" s="15"/>
-      <c r="J255" s="15"/>
-      <c r="K255" s="15"/>
-      <c r="L255" s="15"/>
-      <c r="M255" s="15"/>
-    </row>
-    <row r="256" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A256" s="14" t="s">
-        <v>322</v>
-      </c>
-      <c r="B256" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D256" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="E256" s="15"/>
-      <c r="F256" s="15"/>
-      <c r="G256" s="15"/>
-      <c r="H256" s="15"/>
-      <c r="I256" s="15"/>
-      <c r="J256" s="15"/>
-      <c r="K256" s="15"/>
-      <c r="L256" s="15"/>
-      <c r="M256" s="15"/>
-    </row>
-    <row r="257" spans="1:13" s="7" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A257" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="B257" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D257" s="7" t="s">
-        <v>324</v>
-      </c>
+    <row r="257" spans="1:13" s="9" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="B257" s="26"/>
+      <c r="C257" s="26"/>
+      <c r="D257" s="26"/>
       <c r="E257" s="15"/>
       <c r="F257" s="15"/>
       <c r="G257" s="15"/>
@@ -6272,13 +6272,16 @@
       <c r="L257" s="15"/>
       <c r="M257" s="15"/>
     </row>
-    <row r="258" spans="1:13" s="7" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="23" t="s">
-        <v>280</v>
-      </c>
-      <c r="B258" s="24"/>
-      <c r="C258" s="24"/>
-      <c r="D258" s="24"/>
+    <row r="258" spans="1:13" s="7" customFormat="1" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A258" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="B258" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D258" s="7" t="s">
+        <v>324</v>
+      </c>
       <c r="E258" s="15"/>
       <c r="F258" s="15"/>
       <c r="G258" s="15"/>
@@ -6289,9 +6292,15 @@
       <c r="L258" s="15"/>
       <c r="M258" s="15"/>
     </row>
-    <row r="259" spans="1:13" s="7" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A259" s="14" t="s">
-        <v>201</v>
+        <v>321</v>
+      </c>
+      <c r="B259" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D259" s="7" t="s">
+        <v>355</v>
       </c>
       <c r="E259" s="15"/>
       <c r="F259" s="15"/>
@@ -6303,15 +6312,15 @@
       <c r="L259" s="15"/>
       <c r="M259" s="15"/>
     </row>
-    <row r="260" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" s="7" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A260" s="14" t="s">
-        <v>141</v>
+        <v>322</v>
       </c>
       <c r="B260" s="7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D260" s="7" t="s">
-        <v>360</v>
+        <v>323</v>
       </c>
       <c r="E260" s="15"/>
       <c r="F260" s="15"/>
@@ -6323,13 +6332,13 @@
       <c r="L260" s="15"/>
       <c r="M260" s="15"/>
     </row>
-    <row r="261" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A261" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="B261" s="7" t="s">
-        <v>3</v>
-      </c>
+    <row r="261" spans="1:13" s="7" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="27" t="s">
+        <v>279</v>
+      </c>
+      <c r="B261" s="26"/>
+      <c r="C261" s="26"/>
+      <c r="D261" s="26"/>
       <c r="E261" s="15"/>
       <c r="F261" s="15"/>
       <c r="G261" s="15"/>
@@ -6340,13 +6349,10 @@
       <c r="L261" s="15"/>
       <c r="M261" s="15"/>
     </row>
-    <row r="262" spans="1:13" s="7" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="25" t="s">
-        <v>281</v>
-      </c>
-      <c r="B262" s="24"/>
-      <c r="C262" s="24"/>
-      <c r="D262" s="24"/>
+    <row r="262" spans="1:13" s="7" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A262" s="14" t="s">
+        <v>201</v>
+      </c>
       <c r="E262" s="15"/>
       <c r="F262" s="15"/>
       <c r="G262" s="15"/>
@@ -6357,225 +6363,219 @@
       <c r="L262" s="15"/>
       <c r="M262" s="15"/>
     </row>
-    <row r="263" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A263" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B263" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D263" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="E263" s="15"/>
+      <c r="F263" s="15"/>
+      <c r="G263" s="15"/>
+      <c r="H263" s="15"/>
+      <c r="I263" s="15"/>
+      <c r="J263" s="15"/>
+      <c r="K263" s="15"/>
+      <c r="L263" s="15"/>
+      <c r="M263" s="15"/>
+    </row>
+    <row r="264" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A264" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B264" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E264" s="15"/>
+      <c r="F264" s="15"/>
+      <c r="G264" s="15"/>
+      <c r="H264" s="15"/>
+      <c r="I264" s="15"/>
+      <c r="J264" s="15"/>
+      <c r="K264" s="15"/>
+      <c r="L264" s="15"/>
+      <c r="M264" s="15"/>
+    </row>
+    <row r="265" spans="1:13" s="7" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="B265" s="26"/>
+      <c r="C265" s="26"/>
+      <c r="D265" s="26"/>
+      <c r="E265" s="15"/>
+      <c r="F265" s="15"/>
+      <c r="G265" s="15"/>
+      <c r="H265" s="15"/>
+      <c r="I265" s="15"/>
+      <c r="J265" s="15"/>
+      <c r="K265" s="15"/>
+      <c r="L265" s="15"/>
+      <c r="M265" s="15"/>
+    </row>
+    <row r="266" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A266" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="B263" s="3" t="s">
+      <c r="B266" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D263" s="3" t="s">
+      <c r="D266" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="264" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A264" s="14" t="s">
+    <row r="267" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A267" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B264" s="3" t="s">
+      <c r="B267" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D264" s="3" t="s">
+      <c r="D267" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A268" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D268" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A269" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C269" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A270" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B270" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="271" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A271" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B271" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A272" s="14" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="265" spans="1:13" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A265" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="B265" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D265" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="266" spans="1:13" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A266" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="B266" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C266" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="267" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A267" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="B267" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="268" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A268" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="B268" s="3" t="s">
+      <c r="B272" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="269" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A269" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="B269" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C269" s="3" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="270" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A270" s="14" t="s">
-        <v>365</v>
-      </c>
-      <c r="B270" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D270" s="3" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="271" spans="1:13" s="7" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A271" s="25" t="s">
-        <v>282</v>
-      </c>
-      <c r="B271" s="24"/>
-      <c r="C271" s="24"/>
-      <c r="D271" s="24"/>
-      <c r="E271" s="15"/>
-      <c r="F271" s="15"/>
-      <c r="G271" s="15"/>
-      <c r="H271" s="15"/>
-      <c r="I271" s="15"/>
-      <c r="J271" s="15"/>
-      <c r="K271" s="15"/>
-      <c r="L271" s="15"/>
-      <c r="M271" s="15"/>
-    </row>
-    <row r="272" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A272" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D272" s="3" t="s">
-        <v>220</v>
+      <c r="C272" s="3" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="273" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A273" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="B273" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D273" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" s="7" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="25" t="s">
+        <v>281</v>
+      </c>
+      <c r="B274" s="26"/>
+      <c r="C274" s="26"/>
+      <c r="D274" s="26"/>
+      <c r="E274" s="15"/>
+      <c r="F274" s="15"/>
+      <c r="G274" s="15"/>
+      <c r="H274" s="15"/>
+      <c r="I274" s="15"/>
+      <c r="J274" s="15"/>
+      <c r="K274" s="15"/>
+      <c r="L274" s="15"/>
+      <c r="M274" s="15"/>
+    </row>
+    <row r="275" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A275" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D275" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A276" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B273" s="3" t="s">
+      <c r="B276" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D273" s="3" t="s">
+      <c r="D276" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="274" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A274" s="14" t="s">
+    <row r="277" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A277" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="B274" s="3" t="s">
+      <c r="B277" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="275" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A275" s="14" t="s">
+    <row r="278" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A278" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="B275" s="3" t="s">
+      <c r="B278" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="276" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A276" s="14" t="s">
+    <row r="279" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A279" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="B279" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A280" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="B276" s="3" t="s">
+      <c r="B280" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="277" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A277" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="B277" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="278" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A278" s="14" t="s">
+    <row r="281" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A281" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B278" s="7" t="s">
+      <c r="B281" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="E278" s="15"/>
-      <c r="F278" s="15"/>
-      <c r="G278" s="15"/>
-      <c r="H278" s="15"/>
-      <c r="I278" s="15"/>
-      <c r="J278" s="15"/>
-      <c r="K278" s="15"/>
-      <c r="L278" s="15"/>
-      <c r="M278" s="15"/>
-    </row>
-    <row r="279" spans="1:13" s="8" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A279" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="B279" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C279" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="E279" s="15"/>
-      <c r="F279" s="15"/>
-      <c r="G279" s="15"/>
-      <c r="H279" s="15"/>
-      <c r="I279" s="15"/>
-      <c r="J279" s="15"/>
-      <c r="K279" s="15"/>
-      <c r="L279" s="15"/>
-      <c r="M279" s="15"/>
-    </row>
-    <row r="280" spans="1:13" s="8" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A280" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="B280" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="C280" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="E280" s="15"/>
-      <c r="F280" s="15"/>
-      <c r="G280" s="15"/>
-      <c r="H280" s="15"/>
-      <c r="I280" s="15"/>
-      <c r="J280" s="15"/>
-      <c r="K280" s="15"/>
-      <c r="L280" s="15"/>
-      <c r="M280" s="15"/>
-    </row>
-    <row r="281" spans="1:13" s="7" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A281" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="B281" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C281" s="7" t="s">
-        <v>291</v>
       </c>
       <c r="E281" s="15"/>
       <c r="F281" s="15"/>
@@ -6587,12 +6587,15 @@
       <c r="L281" s="15"/>
       <c r="M281" s="15"/>
     </row>
-    <row r="282" spans="1:13" s="7" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13" s="8" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A282" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="B282" s="7" t="s">
-        <v>61</v>
+        <v>169</v>
+      </c>
+      <c r="B282" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C282" s="8" t="s">
+        <v>402</v>
       </c>
       <c r="E282" s="15"/>
       <c r="F282" s="15"/>
@@ -6604,118 +6607,141 @@
       <c r="L282" s="15"/>
       <c r="M282" s="15"/>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13" s="8" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A283" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="B283" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B283" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C283" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="E283" s="15"/>
+      <c r="F283" s="15"/>
+      <c r="G283" s="15"/>
+      <c r="H283" s="15"/>
+      <c r="I283" s="15"/>
+      <c r="J283" s="15"/>
+      <c r="K283" s="15"/>
+      <c r="L283" s="15"/>
+      <c r="M283" s="15"/>
+    </row>
+    <row r="284" spans="1:13" s="7" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A284" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B284" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C284" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="E284" s="15"/>
+      <c r="F284" s="15"/>
+      <c r="G284" s="15"/>
+      <c r="H284" s="15"/>
+      <c r="I284" s="15"/>
+      <c r="J284" s="15"/>
+      <c r="K284" s="15"/>
+      <c r="L284" s="15"/>
+      <c r="M284" s="15"/>
+    </row>
+    <row r="285" spans="1:13" s="7" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
+      <c r="A285" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B285" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E285" s="15"/>
+      <c r="F285" s="15"/>
+      <c r="G285" s="15"/>
+      <c r="H285" s="15"/>
+      <c r="I285" s="15"/>
+      <c r="J285" s="15"/>
+      <c r="K285" s="15"/>
+      <c r="L285" s="15"/>
+      <c r="M285" s="15"/>
+    </row>
+    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A286" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="B286" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="284" spans="1:13" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A284" s="25" t="s">
-        <v>448</v>
-      </c>
-      <c r="B284" s="24"/>
-      <c r="C284" s="24"/>
-      <c r="D284" s="24"/>
-    </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A285" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="B285" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C285" s="14"/>
-      <c r="D285" s="14"/>
-    </row>
-    <row r="286" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A286" s="14" t="s">
-        <v>449</v>
-      </c>
-      <c r="D286" s="14" t="s">
-        <v>450</v>
-      </c>
-      <c r="E286" s="15"/>
-      <c r="F286" s="15"/>
-      <c r="G286" s="15"/>
-      <c r="H286" s="15"/>
-      <c r="I286" s="15"/>
-      <c r="J286" s="15"/>
-      <c r="K286" s="15"/>
-      <c r="L286" s="15"/>
-      <c r="M286" s="15"/>
-    </row>
-    <row r="287" spans="1:13" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A287" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B287" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C287" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D287" s="14"/>
+    <row r="287" spans="1:13" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A287" s="25" t="s">
+        <v>444</v>
+      </c>
+      <c r="B287" s="26"/>
+      <c r="C287" s="26"/>
+      <c r="D287" s="26"/>
     </row>
     <row r="288" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A288" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B288" s="14" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C288" s="14"/>
       <c r="D288" s="14"/>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A289" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="D289" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="E289" s="15"/>
+      <c r="F289" s="15"/>
+      <c r="G289" s="15"/>
+      <c r="H289" s="15"/>
+      <c r="I289" s="15"/>
+      <c r="J289" s="15"/>
+      <c r="K289" s="15"/>
+      <c r="L289" s="15"/>
+      <c r="M289" s="15"/>
+    </row>
+    <row r="290" spans="1:13" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A290" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B290" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C290" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D290" s="14"/>
+    </row>
+    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A291" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B291" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C291" s="14"/>
+      <c r="D291" s="14"/>
+    </row>
+    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A292" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B289" s="14" t="s">
+      <c r="B292" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C289" s="14"/>
-      <c r="D289" s="14"/>
-    </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A290" s="14" t="s">
+      <c r="C292" s="14"/>
+      <c r="D292" s="14"/>
+    </row>
+    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A293" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="B290" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C290" s="14"/>
-      <c r="D290" s="14"/>
-    </row>
-    <row r="291" spans="1:4" ht="146.25" x14ac:dyDescent="0.25">
-      <c r="A291" s="14" t="s">
-        <v>435</v>
-      </c>
-      <c r="B291" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C291" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D291" s="14"/>
-    </row>
-    <row r="292" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A292" s="14" t="s">
-        <v>436</v>
-      </c>
-      <c r="B292" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C292" s="14" t="s">
-        <v>437</v>
-      </c>
-      <c r="D292" s="14"/>
-    </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A293" s="14" t="s">
-        <v>114</v>
       </c>
       <c r="B293" s="14" t="s">
         <v>3</v>
@@ -6723,16 +6749,50 @@
       <c r="C293" s="14"/>
       <c r="D293" s="14"/>
     </row>
+    <row r="294" spans="1:13" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="A294" s="14" t="s">
+        <v>432</v>
+      </c>
+      <c r="B294" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C294" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D294" s="14"/>
+    </row>
+    <row r="295" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A295" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="B295" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C295" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="D295" s="14"/>
+    </row>
+    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A296" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B296" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C296" s="14"/>
+      <c r="D296" s="14"/>
+    </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A284:D284"/>
-    <mergeCell ref="A258:D258"/>
-    <mergeCell ref="A262:D262"/>
-    <mergeCell ref="A271:D271"/>
+    <mergeCell ref="A287:D287"/>
+    <mergeCell ref="A261:D261"/>
+    <mergeCell ref="A265:D265"/>
+    <mergeCell ref="A274:D274"/>
     <mergeCell ref="A206:D206"/>
-    <mergeCell ref="D241:D242"/>
-    <mergeCell ref="A254:D254"/>
-    <mergeCell ref="D237:D238"/>
+    <mergeCell ref="D244:D245"/>
+    <mergeCell ref="A257:D257"/>
+    <mergeCell ref="D240:D241"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A94:D94"/>

</xml_diff>

<commit_message>
Updates for CITS version 2.35.00
</commit_message>
<xml_diff>
--- a/CITS-WebService/Documentation/APEXA CITS Documentation.xlsx
+++ b/CITS-WebService/Documentation/APEXA CITS Documentation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="165" windowWidth="27795" windowHeight="12525" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TXLife Request" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="457">
   <si>
     <t>ACORD Hierarchy</t>
   </si>
@@ -1076,11 +1076,6 @@
 Each of the AGA/MGA/Carrier parties involved in each contract will be listed.</t>
   </si>
   <si>
-    <t>A reference to the Carrier/MGA/AGA/Company that is signing the contract.
-Will be the APEXA partner entity id prefixed with "P" OR the APEXA contractor entity id prefixed with "C".
-References corresponding  TXLifeResponse/OLifE/Party[N]/@id</t>
-  </si>
-  <si>
     <t>A reference to the individual that signed the contract on behalf of the Signing party.
 Will be the APEXA user entity id prefixed with SIGN.
 References corresponding  TXLifeResponse/OLifE/Party[N]/@id</t>
@@ -1186,12 +1181,6 @@
 Matches the TXLifeResponse/OLifE/Party[N]/@id value above.</t>
   </si>
   <si>
-    <t>Will be the APEXA EntityId prefixed with the letter "O"</t>
-  </si>
-  <si>
-    <t>Will be the APEXA EntityId prefixed with the letters "P"</t>
-  </si>
-  <si>
     <t>Will be the APEXA EntityId prefixed with the letters "CON"</t>
   </si>
   <si>
@@ -1382,12 +1371,6 @@
   </si>
   <si>
     <t>Only included if the contract requires an initial sale to complete.</t>
-  </si>
-  <si>
-    <t>Will be the APEXA EntityId prefixed with the letters "P" for carriers/mgas/agas, "C" for organizations/advisors and "S" for shareholders
-Shareholder id will not be sent unless they have fulfilled the requirement.
-Advisor id will not be sent for company contracts unless they have fulfilled the requirement
-NOT included for the contract requirement itself</t>
   </si>
   <si>
     <t>OLI_PROSTAT_ACTIVE - 1 - Active
@@ -1487,18 +1470,10 @@
     <t>TXLifeResponse/OLifE/Party[1]/Producer/CarrierAppointment[N]/DistributionAgreementInfo[1]/@CheckMailingID</t>
   </si>
   <si>
-    <t>Banking Information - Only sent if advisor as indicated Cheque as the form of payment
-Will be the APEXA Address prefixed with the letters "ADR"
-Same as corresponding TXLifeResponse/OLifE/Address/@id</t>
-  </si>
-  <si>
     <t>Contract Cheque Mailing Address</t>
   </si>
   <si>
     <t>TXLifeResponse/OLifE/Party[1]/Address/@id</t>
-  </si>
-  <si>
-    <t>Will be the APEXA AddressID prefixed with "ADR"</t>
   </si>
   <si>
     <t>TXLifeResponse/OLifE/Party[1]/Producer/CarrierAppointment[N]/ExpDate</t>
@@ -1525,12 +1500,41 @@
 References the contract being transferred.</t>
   </si>
   <si>
-    <t>Points to the AGA ,MGA or Carrier that this contract is with.
-Will be the APEXA EntityId prefixed with the letters "P"</t>
-  </si>
-  <si>
     <t>Points to the AGA, MGA or Carrier that this contract is with.  In the case of multi-level contracts it is the highest tier (Carrier &gt; MGA &gt; AGA)
 Will be the APEXA EntityId prefixed with the letters "P"</t>
+  </si>
+  <si>
+    <t>Will be the APEXA EntityId prefixed with the letter "S"</t>
+  </si>
+  <si>
+    <t>Will be the APEXA EntityId prefixed with the letters "C"</t>
+  </si>
+  <si>
+    <t>Points to the AGA ,MGA or Carrier that this contract is with.
+Will be the APEXA EntityId prefixed with the letters "C"</t>
+  </si>
+  <si>
+    <t>Will be the APEXA EntityId prefixed with the letters "C" for carriers/mgas/agas/organizations/advisors and "S" for shareholders
+Shareholder id will not be sent unless they have fulfilled the requirement.
+Advisor id will not be sent for company contracts unless they have fulfilled the requirement
+NOT included for the contract requirement itself</t>
+  </si>
+  <si>
+    <t>A reference to the Carrier/MGA/AGA/Company that is signing the contract.
+Will be the APEXA entity id prefixed with "C".
+References corresponding  TXLifeResponse/OLifE/Party[N]/@id</t>
+  </si>
+  <si>
+    <t>Will be the APEXA AddressID prefixed with "ADRBUS" for Business Address, "ADRRES" for Residential Address and "ADR" for all other address types.</t>
+  </si>
+  <si>
+    <t>Banking Information - Only sent if advisor as indicated Cheque as the form of payment
+Will be the APEXA AddressID prefixed with "ADRBUS" for Business Address, "ADRRES" for Residential Address and "ADR" for all other address types.
+Same as corresponding TXLifeResponse/OLifE/Address/@id</t>
+  </si>
+  <si>
+    <t>Will be the APEXA EntityId prefixed with the letters "TRF"
+References the contract being transferred.</t>
   </si>
 </sst>
 </file>
@@ -1994,7 +1998,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2047,16 +2051,25 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2068,13 +2081,10 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2475,60 +2485,60 @@
         <v>89</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>179</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="6" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>334</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="12" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="12" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>250</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
@@ -2540,7 +2550,7 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2932,12 +2942,12 @@
       </c>
     </row>
     <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
     </row>
     <row r="8" spans="1:4" s="11" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -2974,7 +2984,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>10</v>
@@ -3006,19 +3016,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M296"/>
+  <dimension ref="A1:M297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D172" sqref="D172"/>
+    <sheetView tabSelected="1" topLeftCell="B201" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E219" sqref="E219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="78.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="103.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="93.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="74.42578125" style="3" customWidth="1"/>
     <col min="5" max="13" width="9.140625" style="15"/>
     <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -3056,7 +3067,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
@@ -3113,12 +3124,12 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
@@ -3139,7 +3150,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="22.5" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3171,8 +3182,8 @@
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="24" t="s">
-        <v>406</v>
+      <c r="D13" s="27" t="s">
+        <v>403</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -3192,9 +3203,9 @@
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="D14" s="24"/>
+        <v>402</v>
+      </c>
+      <c r="D14" s="27"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
@@ -3212,7 +3223,7 @@
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="27" t="s">
         <v>181</v>
       </c>
       <c r="E15" s="15"/>
@@ -3232,7 +3243,7 @@
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="23"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
@@ -3253,7 +3264,7 @@
       <c r="C17" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D17" s="23"/>
+      <c r="D17" s="26"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -3331,7 +3342,7 @@
         <v>104</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="26" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -3369,7 +3380,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="30" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3383,12 +3394,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="14" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="14" customFormat="1" ht="22.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -3437,7 +3448,7 @@
     </row>
     <row r="36" spans="1:13" ht="146.25" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>55</v>
@@ -3448,13 +3459,13 @@
     </row>
     <row r="37" spans="1:13" s="14" customFormat="1" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -3499,24 +3510,24 @@
     </row>
     <row r="40" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="41" spans="1:13" s="14" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B41" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
@@ -3544,7 +3555,7 @@
         <v>21</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="44" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -3565,7 +3576,7 @@
     </row>
     <row r="46" spans="1:13" s="14" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>3</v>
@@ -3604,7 +3615,7 @@
         <v>22</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="50" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -3623,7 +3634,7 @@
         <v>10</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="E51" s="15"/>
       <c r="F51" s="15"/>
@@ -3643,7 +3654,7 @@
         <v>69</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E52" s="15"/>
       <c r="F52" s="15"/>
@@ -3703,7 +3714,7 @@
         <v>61</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E55" s="15"/>
       <c r="F55" s="15"/>
@@ -3717,7 +3728,7 @@
     </row>
     <row r="56" spans="1:13" s="14" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>3</v>
@@ -3753,7 +3764,7 @@
     </row>
     <row r="59" spans="1:13" s="14" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>23</v>
@@ -3797,12 +3808,12 @@
       <c r="M61" s="15"/>
     </row>
     <row r="62" spans="1:13" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
+      <c r="A62" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B62" s="19"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
     </row>
     <row r="63" spans="1:13" ht="33.75" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
@@ -3828,13 +3839,13 @@
     </row>
     <row r="65" spans="1:13" s="14" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B65" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="66" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -3849,12 +3860,12 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="18" t="s">
+      <c r="A67" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B67" s="19"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="19"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
     </row>
     <row r="68" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
@@ -3864,18 +3875,18 @@
         <v>10</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="69" spans="1:13" s="11" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B69" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E69" s="15"/>
       <c r="F69" s="15"/>
@@ -3895,7 +3906,7 @@
         <v>12</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="71" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -3906,18 +3917,18 @@
         <v>3</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="72" spans="1:13" s="14" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B72" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="146.25" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -3945,7 +3956,7 @@
         <v>54</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="75" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -3956,18 +3967,18 @@
         <v>12</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="76" spans="1:13" s="14" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B76" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="E76" s="15"/>
       <c r="F76" s="15"/>
@@ -3980,12 +3991,12 @@
       <c r="M76" s="15"/>
     </row>
     <row r="77" spans="1:13" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="18" t="s">
+      <c r="A77" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B77" s="19"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="19"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
     </row>
     <row r="78" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
@@ -4009,7 +4020,7 @@
         <v>75</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="80" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4031,7 +4042,7 @@
         <v>3</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="82" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4042,16 +4053,16 @@
         <v>12</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="18" t="s">
+      <c r="A83" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B83" s="19"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="19"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
     </row>
     <row r="84" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
@@ -4089,7 +4100,7 @@
         <v>10</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="87" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4104,12 +4115,12 @@
       </c>
     </row>
     <row r="88" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="18" t="s">
+      <c r="A88" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="21"/>
     </row>
     <row r="89" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
@@ -4164,12 +4175,12 @@
       </c>
     </row>
     <row r="94" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="18" t="s">
+      <c r="A94" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B94" s="19"/>
-      <c r="C94" s="19"/>
-      <c r="D94" s="19"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="21"/>
     </row>
     <row r="95" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
@@ -4190,7 +4201,7 @@
         <v>11</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="97" spans="1:4" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4277,7 +4288,7 @@
         <v>11</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4288,7 +4299,7 @@
         <v>23</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4299,7 +4310,7 @@
         <v>23</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="108" spans="1:4" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4336,12 +4347,12 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="18" t="s">
+      <c r="A111" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B111" s="19"/>
-      <c r="C111" s="19"/>
-      <c r="D111" s="19"/>
+      <c r="B111" s="21"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="21"/>
     </row>
     <row r="112" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
@@ -4389,7 +4400,7 @@
         <v>3</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="117" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4400,7 +4411,7 @@
         <v>3</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="118" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4422,7 +4433,7 @@
         <v>65</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="120" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4433,7 +4444,7 @@
         <v>12</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="121" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4444,7 +4455,7 @@
         <v>12</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="122" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4455,7 +4466,7 @@
         <v>12</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="123" spans="1:13" ht="45" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4469,7 +4480,7 @@
         <v>72</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="124" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4480,7 +4491,7 @@
         <v>10</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="125" spans="1:13" s="2" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4491,7 +4502,7 @@
         <v>69</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E125" s="15"/>
       <c r="F125" s="15"/>
@@ -4544,7 +4555,7 @@
     </row>
     <row r="129" spans="1:13" s="14" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B129" s="14" t="s">
         <v>3</v>
@@ -4601,12 +4612,12 @@
       </c>
     </row>
     <row r="134" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A134" s="18" t="s">
+      <c r="A134" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B134" s="19"/>
-      <c r="C134" s="19"/>
-      <c r="D134" s="19"/>
+      <c r="B134" s="21"/>
+      <c r="C134" s="21"/>
+      <c r="D134" s="21"/>
     </row>
     <row r="135" spans="1:13" s="2" customFormat="1" ht="22.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
@@ -4636,7 +4647,7 @@
         <v>11</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E136" s="15"/>
       <c r="F136" s="15"/>
@@ -4670,7 +4681,7 @@
         <v>60</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="139" spans="1:13" s="11" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -4681,7 +4692,7 @@
         <v>59</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="E139" s="15"/>
       <c r="F139" s="15"/>
@@ -4695,16 +4706,16 @@
     </row>
     <row r="140" spans="1:13" s="11" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B140" s="11" t="s">
         <v>250</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="E140" s="15"/>
       <c r="F140" s="15"/>
@@ -4718,13 +4729,13 @@
     </row>
     <row r="141" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>250</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="142" spans="1:13" s="7" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4755,7 +4766,7 @@
         <v>11</v>
       </c>
       <c r="D143" s="7" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E143" s="15"/>
       <c r="F143" s="15"/>
@@ -4775,7 +4786,7 @@
         <v>23</v>
       </c>
       <c r="D144" s="7" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E144" s="15"/>
       <c r="F144" s="15"/>
@@ -4795,7 +4806,7 @@
         <v>23</v>
       </c>
       <c r="D145" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E145" s="15"/>
       <c r="F145" s="15"/>
@@ -4868,12 +4879,12 @@
       <c r="M148" s="15"/>
     </row>
     <row r="149" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A149" s="18" t="s">
-        <v>396</v>
-      </c>
-      <c r="B149" s="19"/>
-      <c r="C149" s="19"/>
-      <c r="D149" s="19"/>
+      <c r="A149" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="B149" s="21"/>
+      <c r="C149" s="21"/>
+      <c r="D149" s="21"/>
     </row>
     <row r="150" spans="1:13" ht="22.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A150" s="15" t="s">
@@ -4883,7 +4894,7 @@
         <v>10</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="151" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -4964,7 +4975,7 @@
         <v>3</v>
       </c>
       <c r="D156" s="7" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E156" s="15"/>
       <c r="F156" s="15"/>
@@ -4984,7 +4995,7 @@
         <v>65</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="158" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4994,7 +5005,7 @@
       <c r="B158" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D158" s="22" t="s">
+      <c r="D158" s="25" t="s">
         <v>193</v>
       </c>
     </row>
@@ -5005,7 +5016,7 @@
       <c r="B159" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D159" s="23"/>
+      <c r="D159" s="26"/>
     </row>
     <row r="160" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A160" s="15" t="s">
@@ -5017,7 +5028,7 @@
       <c r="C160" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D160" s="23"/>
+      <c r="D160" s="26"/>
     </row>
     <row r="161" spans="1:13" ht="11.25" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A161" s="15" t="s">
@@ -5026,7 +5037,7 @@
       <c r="B161" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D161" s="23"/>
+      <c r="D161" s="26"/>
     </row>
     <row r="162" spans="1:13" s="6" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A162" s="15" t="s">
@@ -5056,7 +5067,7 @@
         <v>11</v>
       </c>
       <c r="D163" s="7" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E163" s="15"/>
       <c r="F163" s="15"/>
@@ -5096,7 +5107,7 @@
         <v>23</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="E165" s="15"/>
       <c r="F165" s="15"/>
@@ -5172,12 +5183,12 @@
       <c r="M168" s="15"/>
     </row>
     <row r="169" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A169" s="18" t="s">
+      <c r="A169" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B169" s="19"/>
-      <c r="C169" s="19"/>
-      <c r="D169" s="19"/>
+      <c r="B169" s="21"/>
+      <c r="C169" s="21"/>
+      <c r="D169" s="21"/>
     </row>
     <row r="170" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
@@ -5198,7 +5209,7 @@
         <v>11</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="172" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5239,7 +5250,7 @@
         <v>11</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="176" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5250,7 +5261,7 @@
         <v>23</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5261,7 +5272,7 @@
         <v>23</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="178" spans="1:4" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5298,20 +5309,20 @@
       </c>
     </row>
     <row r="181" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A181" s="18" t="s">
+      <c r="A181" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B181" s="19"/>
-      <c r="C181" s="19"/>
-      <c r="D181" s="19"/>
+      <c r="B181" s="21"/>
+      <c r="C181" s="21"/>
+      <c r="D181" s="21"/>
     </row>
     <row r="182" spans="1:4" s="14" customFormat="1" ht="42.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="20" t="s">
+      <c r="A182" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="B182" s="21"/>
-      <c r="C182" s="21"/>
-      <c r="D182" s="21"/>
+      <c r="B182" s="29"/>
+      <c r="C182" s="29"/>
+      <c r="D182" s="29"/>
     </row>
     <row r="183" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A183" s="14" t="s">
@@ -5332,7 +5343,7 @@
         <v>11</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -5343,7 +5354,7 @@
         <v>23</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -5354,7 +5365,7 @@
         <v>23</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="187" spans="1:4" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -5387,7 +5398,7 @@
         <v>35</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="190" spans="1:4" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -5402,12 +5413,12 @@
       </c>
     </row>
     <row r="191" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A191" s="18" t="s">
-        <v>332</v>
-      </c>
-      <c r="B191" s="19"/>
-      <c r="C191" s="19"/>
-      <c r="D191" s="19"/>
+      <c r="A191" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="B191" s="21"/>
+      <c r="C191" s="21"/>
+      <c r="D191" s="21"/>
     </row>
     <row r="192" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A192" s="14" t="s">
@@ -5428,7 +5439,7 @@
         <v>11</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="194" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5439,7 +5450,7 @@
         <v>23</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="195" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5450,7 +5461,7 @@
         <v>23</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="196" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5483,7 +5494,7 @@
         <v>35</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="199" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5516,7 +5527,7 @@
         <v>11</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>354</v>
+        <v>449</v>
       </c>
     </row>
     <row r="202" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5527,7 +5538,7 @@
         <v>7</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="203" spans="1:13" s="11" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5549,7 +5560,7 @@
     </row>
     <row r="204" spans="1:13" s="11" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A204" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B204" s="11" t="s">
         <v>10</v>
@@ -5566,19 +5577,19 @@
     </row>
     <row r="205" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A205" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="206" spans="1:13" s="7" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="18" t="s">
+      <c r="A206" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="B206" s="19"/>
-      <c r="C206" s="19"/>
-      <c r="D206" s="19"/>
+      <c r="B206" s="21"/>
+      <c r="C206" s="21"/>
+      <c r="D206" s="21"/>
       <c r="E206" s="15"/>
       <c r="F206" s="15"/>
       <c r="G206" s="15"/>
@@ -5614,7 +5625,7 @@
         <v>11</v>
       </c>
       <c r="D208" s="7" t="s">
-        <v>355</v>
+        <v>450</v>
       </c>
       <c r="E208" s="15"/>
       <c r="F208" s="15"/>
@@ -5687,14 +5698,14 @@
       <c r="M211" s="15"/>
     </row>
     <row r="212" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A212" s="18" t="s">
+      <c r="A212" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="B212" s="19"/>
-      <c r="C212" s="19"/>
-      <c r="D212" s="19"/>
-    </row>
-    <row r="213" spans="1:13" s="8" customFormat="1" ht="22.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B212" s="21"/>
+      <c r="C212" s="21"/>
+      <c r="D212" s="21"/>
+    </row>
+    <row r="213" spans="1:13" s="8" customFormat="1" ht="33.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A213" s="15" t="s">
         <v>230</v>
       </c>
@@ -5719,7 +5730,7 @@
         <v>231</v>
       </c>
       <c r="D214" s="7" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E214" s="15"/>
       <c r="F214" s="15"/>
@@ -5731,12 +5742,12 @@
       <c r="L214" s="15"/>
       <c r="M214" s="15"/>
     </row>
-    <row r="215" spans="1:13" s="8" customFormat="1" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" s="8" customFormat="1" ht="33.75" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A215" s="15" t="s">
         <v>263</v>
       </c>
       <c r="D215" s="7" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="E215" s="15"/>
       <c r="F215" s="15"/>
@@ -5753,7 +5764,7 @@
         <v>264</v>
       </c>
       <c r="D216" s="15" t="s">
-        <v>355</v>
+        <v>450</v>
       </c>
     </row>
     <row r="217" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5786,7 +5797,7 @@
         <v>23</v>
       </c>
       <c r="D219" s="15" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="220" spans="1:13" s="15" customFormat="1" ht="67.5" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5797,10 +5808,10 @@
         <v>185</v>
       </c>
       <c r="C220" s="15" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D220" s="15" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="221" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5816,7 +5827,7 @@
     </row>
     <row r="222" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A222" s="15" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="B222" s="15" t="s">
         <v>12</v>
@@ -5844,23 +5855,23 @@
         <v>23</v>
       </c>
       <c r="D224" s="15" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="225" spans="1:13" s="17" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A225" s="17" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="B225" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D225" s="16" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="226" spans="1:13" s="17" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A226" s="17" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="B226" s="17" t="s">
         <v>3</v>
@@ -5871,27 +5882,27 @@
     </row>
     <row r="227" spans="1:13" s="17" customFormat="1" ht="67.5" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A227" s="17" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="B227" s="17" t="s">
         <v>185</v>
       </c>
       <c r="C227" s="17" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D227" s="17" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="228" spans="1:13" s="17" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A228" s="17" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="B228" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D228" s="17" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
     <row r="229" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5913,7 +5924,7 @@
         <v>23</v>
       </c>
       <c r="D230" s="15" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="231" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -5940,18 +5951,18 @@
     </row>
     <row r="233" spans="1:13" s="15" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A233" s="15" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B233" s="15" t="s">
         <v>10</v>
       </c>
       <c r="D233" s="15" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="234" spans="1:13" s="15" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A234" s="15" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B234" s="15" t="s">
         <v>3</v>
@@ -5959,13 +5970,13 @@
     </row>
     <row r="235" spans="1:13" s="15" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A235" s="15" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B235" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C235" s="15" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="236" spans="1:13" s="2" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
@@ -6005,15 +6016,15 @@
       <c r="L237" s="15"/>
       <c r="M237" s="15"/>
     </row>
-    <row r="238" spans="1:13" s="15" customFormat="1" ht="33.75" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" s="15" customFormat="1" ht="45" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A238" s="15" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B238" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D238" s="15" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
     </row>
     <row r="239" spans="1:13" s="2" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -6043,8 +6054,8 @@
       <c r="B240" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D240" s="24" t="s">
-        <v>416</v>
+      <c r="D240" s="27" t="s">
+        <v>413</v>
       </c>
       <c r="E240" s="15"/>
       <c r="F240" s="15"/>
@@ -6058,15 +6069,15 @@
     </row>
     <row r="241" spans="1:13" s="13" customFormat="1" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A241" s="15" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B241" s="13" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C241" s="13" t="s">
-        <v>415</v>
-      </c>
-      <c r="D241" s="23"/>
+        <v>412</v>
+      </c>
+      <c r="D241" s="26"/>
       <c r="E241" s="15"/>
       <c r="F241" s="15"/>
       <c r="G241" s="15"/>
@@ -6088,7 +6099,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="243" spans="1:13" ht="45" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" ht="56.25" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A243" s="15" t="s">
         <v>236</v>
       </c>
@@ -6096,7 +6107,7 @@
         <v>23</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>417</v>
+        <v>452</v>
       </c>
     </row>
     <row r="244" spans="1:13" ht="11.25" customHeight="1" outlineLevel="3" x14ac:dyDescent="0.25">
@@ -6106,7 +6117,7 @@
       <c r="B244" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D244" s="22" t="s">
+      <c r="D244" s="25" t="s">
         <v>218</v>
       </c>
     </row>
@@ -6117,7 +6128,7 @@
       <c r="B245" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D245" s="23"/>
+      <c r="D245" s="26"/>
     </row>
     <row r="246" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A246" s="15" t="s">
@@ -6155,7 +6166,7 @@
         <v>69</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D248" s="2" t="s">
         <v>70</v>
@@ -6191,7 +6202,7 @@
     </row>
     <row r="251" spans="1:13" s="14" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A251" s="15" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B251" s="14" t="s">
         <v>3</v>
@@ -6225,18 +6236,18 @@
         <v>23</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>325</v>
+        <v>453</v>
       </c>
     </row>
     <row r="254" spans="1:13" ht="33.75" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A254" s="15" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B254" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="255" spans="1:13" ht="22.5" outlineLevel="4" x14ac:dyDescent="0.25">
@@ -6256,12 +6267,12 @@
       </c>
     </row>
     <row r="257" spans="1:13" s="9" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="25" t="s">
+      <c r="A257" s="22" t="s">
         <v>298</v>
       </c>
-      <c r="B257" s="26"/>
-      <c r="C257" s="26"/>
-      <c r="D257" s="26"/>
+      <c r="B257" s="23"/>
+      <c r="C257" s="23"/>
+      <c r="D257" s="23"/>
       <c r="E257" s="15"/>
       <c r="F257" s="15"/>
       <c r="G257" s="15"/>
@@ -6300,7 +6311,7 @@
         <v>23</v>
       </c>
       <c r="D259" s="7" t="s">
-        <v>355</v>
+        <v>450</v>
       </c>
       <c r="E259" s="15"/>
       <c r="F259" s="15"/>
@@ -6333,12 +6344,12 @@
       <c r="M260" s="15"/>
     </row>
     <row r="261" spans="1:13" s="7" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="27" t="s">
+      <c r="A261" s="24" t="s">
         <v>279</v>
       </c>
-      <c r="B261" s="26"/>
-      <c r="C261" s="26"/>
-      <c r="D261" s="26"/>
+      <c r="B261" s="23"/>
+      <c r="C261" s="23"/>
+      <c r="D261" s="23"/>
       <c r="E261" s="15"/>
       <c r="F261" s="15"/>
       <c r="G261" s="15"/>
@@ -6371,7 +6382,7 @@
         <v>11</v>
       </c>
       <c r="D263" s="7" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E263" s="15"/>
       <c r="F263" s="15"/>
@@ -6400,163 +6411,175 @@
       <c r="L264" s="15"/>
       <c r="M264" s="15"/>
     </row>
-    <row r="265" spans="1:13" s="7" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="25" t="s">
+    <row r="265" spans="1:13" s="18" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A265" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B265" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C265" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="E265" s="19"/>
+      <c r="F265" s="19"/>
+      <c r="G265" s="19"/>
+      <c r="H265" s="19"/>
+      <c r="I265" s="19"/>
+      <c r="J265" s="19"/>
+      <c r="K265" s="19"/>
+      <c r="L265" s="19"/>
+      <c r="M265" s="19"/>
+    </row>
+    <row r="266" spans="1:13" s="7" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="B265" s="26"/>
-      <c r="C265" s="26"/>
-      <c r="D265" s="26"/>
-      <c r="E265" s="15"/>
-      <c r="F265" s="15"/>
-      <c r="G265" s="15"/>
-      <c r="H265" s="15"/>
-      <c r="I265" s="15"/>
-      <c r="J265" s="15"/>
-      <c r="K265" s="15"/>
-      <c r="L265" s="15"/>
-      <c r="M265" s="15"/>
-    </row>
-    <row r="266" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A266" s="14" t="s">
+      <c r="B266" s="23"/>
+      <c r="C266" s="23"/>
+      <c r="D266" s="23"/>
+      <c r="E266" s="15"/>
+      <c r="F266" s="15"/>
+      <c r="G266" s="15"/>
+      <c r="H266" s="15"/>
+      <c r="I266" s="15"/>
+      <c r="J266" s="15"/>
+      <c r="K266" s="15"/>
+      <c r="L266" s="15"/>
+      <c r="M266" s="15"/>
+    </row>
+    <row r="267" spans="1:13" ht="22.5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A267" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="B266" s="3" t="s">
+      <c r="B267" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D266" s="3" t="s">
+      <c r="D267" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="267" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A267" s="14" t="s">
+    <row r="268" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A268" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B267" s="3" t="s">
+      <c r="B268" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D267" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="268" spans="1:13" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A268" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="B268" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D268" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="269" spans="1:13" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A269" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D269" s="3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" ht="22.5" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A270" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="B269" s="3" t="s">
+      <c r="B270" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C269" s="3" t="s">
+      <c r="C270" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="270" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A270" s="14" t="s">
+    <row r="271" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A271" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="B270" s="3" t="s">
+      <c r="B271" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="271" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A271" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="B271" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="272" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A272" s="14" t="s">
-        <v>361</v>
+        <v>175</v>
       </c>
       <c r="B272" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C272" s="3" t="s">
-        <v>363</v>
-      </c>
     </row>
     <row r="273" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A273" s="14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B273" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D273" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="274" spans="1:13" s="7" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A274" s="25" t="s">
+      <c r="C273" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A274" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="B274" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D274" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" s="7" customFormat="1" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A275" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="B274" s="26"/>
-      <c r="C274" s="26"/>
-      <c r="D274" s="26"/>
-      <c r="E274" s="15"/>
-      <c r="F274" s="15"/>
-      <c r="G274" s="15"/>
-      <c r="H274" s="15"/>
-      <c r="I274" s="15"/>
-      <c r="J274" s="15"/>
-      <c r="K274" s="15"/>
-      <c r="L274" s="15"/>
-      <c r="M274" s="15"/>
-    </row>
-    <row r="275" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A275" s="14" t="s">
+      <c r="B275" s="23"/>
+      <c r="C275" s="23"/>
+      <c r="D275" s="23"/>
+      <c r="E275" s="15"/>
+      <c r="F275" s="15"/>
+      <c r="G275" s="15"/>
+      <c r="H275" s="15"/>
+      <c r="I275" s="15"/>
+      <c r="J275" s="15"/>
+      <c r="K275" s="15"/>
+      <c r="L275" s="15"/>
+      <c r="M275" s="15"/>
+    </row>
+    <row r="276" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A276" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="B275" s="3" t="s">
+      <c r="B276" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D275" s="3" t="s">
+      <c r="D276" s="3" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="276" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A276" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B276" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D276" s="3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="277" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A277" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B277" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D277" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A278" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="B277" s="3" t="s">
+      <c r="B278" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="278" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
-      <c r="A278" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="B278" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="279" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A279" s="14" t="s">
-        <v>302</v>
+        <v>188</v>
       </c>
       <c r="B279" s="3" t="s">
         <v>3</v>
@@ -6564,38 +6587,26 @@
     </row>
     <row r="280" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A280" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B280" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:13" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A281" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B281" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" s="7" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
+      <c r="A282" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B281" s="7" t="s">
+      <c r="B282" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="E281" s="15"/>
-      <c r="F281" s="15"/>
-      <c r="G281" s="15"/>
-      <c r="H281" s="15"/>
-      <c r="I281" s="15"/>
-      <c r="J281" s="15"/>
-      <c r="K281" s="15"/>
-      <c r="L281" s="15"/>
-      <c r="M281" s="15"/>
-    </row>
-    <row r="282" spans="1:13" s="8" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
-      <c r="A282" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="B282" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C282" s="8" t="s">
-        <v>402</v>
       </c>
       <c r="E282" s="15"/>
       <c r="F282" s="15"/>
@@ -6607,15 +6618,15 @@
       <c r="L282" s="15"/>
       <c r="M282" s="15"/>
     </row>
-    <row r="283" spans="1:13" s="8" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13" s="8" customFormat="1" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A283" s="14" t="s">
-        <v>255</v>
+        <v>169</v>
       </c>
       <c r="B283" s="8" t="s">
-        <v>253</v>
+        <v>69</v>
       </c>
       <c r="C283" s="8" t="s">
-        <v>289</v>
+        <v>399</v>
       </c>
       <c r="E283" s="15"/>
       <c r="F283" s="15"/>
@@ -6627,15 +6638,15 @@
       <c r="L283" s="15"/>
       <c r="M283" s="15"/>
     </row>
-    <row r="284" spans="1:13" s="7" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:13" s="8" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A284" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="B284" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C284" s="7" t="s">
-        <v>290</v>
+        <v>255</v>
+      </c>
+      <c r="B284" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C284" s="8" t="s">
+        <v>289</v>
       </c>
       <c r="E284" s="15"/>
       <c r="F284" s="15"/>
@@ -6649,10 +6660,13 @@
     </row>
     <row r="285" spans="1:13" s="7" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A285" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B285" s="7" t="s">
-        <v>61</v>
+        <v>68</v>
+      </c>
+      <c r="C285" s="7" t="s">
+        <v>290</v>
       </c>
       <c r="E285" s="15"/>
       <c r="F285" s="15"/>
@@ -6664,74 +6678,81 @@
       <c r="L285" s="15"/>
       <c r="M285" s="15"/>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:13" s="7" customFormat="1" outlineLevel="4" x14ac:dyDescent="0.25">
       <c r="A286" s="14" t="s">
-        <v>429</v>
-      </c>
-      <c r="B286" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B286" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E286" s="15"/>
+      <c r="F286" s="15"/>
+      <c r="G286" s="15"/>
+      <c r="H286" s="15"/>
+      <c r="I286" s="15"/>
+      <c r="J286" s="15"/>
+      <c r="K286" s="15"/>
+      <c r="L286" s="15"/>
+      <c r="M286" s="15"/>
+    </row>
+    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A287" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="B287" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:13" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A287" s="25" t="s">
-        <v>444</v>
-      </c>
-      <c r="B287" s="26"/>
-      <c r="C287" s="26"/>
-      <c r="D287" s="26"/>
-    </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A288" s="14" t="s">
+    <row r="288" spans="1:13" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A288" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B288" s="23"/>
+      <c r="C288" s="23"/>
+      <c r="D288" s="23"/>
+    </row>
+    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A289" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B288" s="14" t="s">
+      <c r="B289" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C288" s="14"/>
-      <c r="D288" s="14"/>
-    </row>
-    <row r="289" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A289" s="14" t="s">
-        <v>445</v>
-      </c>
-      <c r="D289" s="14" t="s">
-        <v>446</v>
-      </c>
-      <c r="E289" s="15"/>
-      <c r="F289" s="15"/>
-      <c r="G289" s="15"/>
-      <c r="H289" s="15"/>
-      <c r="I289" s="15"/>
-      <c r="J289" s="15"/>
-      <c r="K289" s="15"/>
-      <c r="L289" s="15"/>
-      <c r="M289" s="15"/>
-    </row>
-    <row r="290" spans="1:13" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="C289" s="14"/>
+      <c r="D289" s="14"/>
+    </row>
+    <row r="290" spans="1:13" s="14" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A290" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="D290" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="E290" s="15"/>
+      <c r="F290" s="15"/>
+      <c r="G290" s="15"/>
+      <c r="H290" s="15"/>
+      <c r="I290" s="15"/>
+      <c r="J290" s="15"/>
+      <c r="K290" s="15"/>
+      <c r="L290" s="15"/>
+      <c r="M290" s="15"/>
+    </row>
+    <row r="291" spans="1:13" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A291" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B290" s="14" t="s">
+      <c r="B291" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C290" s="14" t="s">
+      <c r="C291" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D290" s="14"/>
-    </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A291" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B291" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C291" s="14"/>
       <c r="D291" s="14"/>
     </row>
     <row r="292" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A292" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B292" s="14" t="s">
         <v>3</v>
@@ -6741,7 +6762,7 @@
     </row>
     <row r="293" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A293" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B293" s="14" t="s">
         <v>3</v>
@@ -6749,50 +6770,61 @@
       <c r="C293" s="14"/>
       <c r="D293" s="14"/>
     </row>
-    <row r="294" spans="1:13" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A294" s="14" t="s">
-        <v>432</v>
+        <v>113</v>
       </c>
       <c r="B294" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C294" s="14"/>
+      <c r="D294" s="14"/>
+    </row>
+    <row r="295" spans="1:13" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="A295" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="B295" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C294" s="14" t="s">
+      <c r="C295" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D294" s="14"/>
-    </row>
-    <row r="295" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A295" s="14" t="s">
-        <v>433</v>
-      </c>
-      <c r="B295" s="14" t="s">
+      <c r="D295" s="14"/>
+    </row>
+    <row r="296" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A296" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="B296" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C295" s="14" t="s">
-        <v>434</v>
-      </c>
-      <c r="D295" s="14"/>
-    </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A296" s="14" t="s">
+      <c r="C296" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="D296" s="14"/>
+    </row>
+    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A297" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B296" s="14" t="s">
+      <c r="B297" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C296" s="14"/>
-      <c r="D296" s="14"/>
+      <c r="C297" s="14"/>
+      <c r="D297" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A287:D287"/>
-    <mergeCell ref="A261:D261"/>
-    <mergeCell ref="A265:D265"/>
-    <mergeCell ref="A274:D274"/>
-    <mergeCell ref="A206:D206"/>
-    <mergeCell ref="D244:D245"/>
-    <mergeCell ref="A257:D257"/>
-    <mergeCell ref="D240:D241"/>
+    <mergeCell ref="A182:D182"/>
+    <mergeCell ref="A191:D191"/>
+    <mergeCell ref="A212:D212"/>
+    <mergeCell ref="A169:D169"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A181:D181"/>
+    <mergeCell ref="A149:D149"/>
+    <mergeCell ref="D158:D161"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A94:D94"/>
@@ -6802,17 +6834,17 @@
     <mergeCell ref="A62:D62"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="A88:D88"/>
-    <mergeCell ref="A182:D182"/>
-    <mergeCell ref="A191:D191"/>
-    <mergeCell ref="A212:D212"/>
-    <mergeCell ref="A169:D169"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A181:D181"/>
-    <mergeCell ref="A149:D149"/>
-    <mergeCell ref="D158:D161"/>
+    <mergeCell ref="A288:D288"/>
+    <mergeCell ref="A261:D261"/>
+    <mergeCell ref="A266:D266"/>
+    <mergeCell ref="A275:D275"/>
+    <mergeCell ref="A206:D206"/>
+    <mergeCell ref="D244:D245"/>
+    <mergeCell ref="A257:D257"/>
+    <mergeCell ref="D240:D241"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>